<commit_message>
updates to publisher to save schematron.zip
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-us-core-questionnaireresponse.xlsx
+++ b/docs/StructureDefinition-us-core-questionnaireresponse.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$68</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="414">
   <si>
     <t>Property</t>
   </si>
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/healthedata1-sandbox/StructureDefinition/us-core-questionnaireresponse</t>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</t>
   </si>
   <si>
     <t>Version</t>
@@ -618,17 +618,6 @@
     <t>Tags that a provider may use in their workflow to indicate/categorize that the context of this Questionnaire Response relates to Social Determinants of Health.</t>
   </si>
   <si>
-    <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
-  &lt;code value="sdoh"/&gt;
-&lt;/valueCoding&gt;</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>http://www.fhir.org/guides/healthedata1-sandbox/ValueSet/temp</t>
-  </si>
-  <si>
     <t>QuestionnaireResponse.implicitRules</t>
   </si>
   <si>
@@ -911,16 +900,10 @@
     <t>url</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://www.fhir.org/guides/argonaut/argo-write/StructureDefinition/questionnaire-url}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/core/StructureDefinition/questionnaire-url}
 </t>
   </si>
   <si>
-    <t>The location where a non-FHIR questionnaire/survey form can be found.</t>
-  </si>
-  <si>
-    <t>This extension is used when the survey,form, or questionnaire which is being anwered is not a FHIR [Questionnaire](https://www.hl7.org/fhir/questionnaire.html), otherwise the [canonical url](https://www.hl7.org/fhir/questionnaire.html#canonical) for the FHIR Questionnaire is used.</t>
-  </si>
-  <si>
     <t>QuestionnaireResponse.questionnaire.value</t>
   </si>
   <si>
@@ -943,6 +926,9 @@
   </si>
   <si>
     <t>The information on Questionnaire resources  may possibly be gathered during multiple sessions and altered after considered being finished.</t>
+  </si>
+  <si>
+    <t>required</t>
   </si>
   <si>
     <t>Lifecycle status of the questionnaire response.</t>
@@ -1637,7 +1623,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL61"/>
+  <dimension ref="A1:AL68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1656,7 +1642,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="65.73046875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="58.7265625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1670,7 +1656,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.22265625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="60.92578125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="59.421875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
@@ -3789,7 +3775,7 @@
         <v>76</v>
       </c>
       <c r="R20" t="s" s="2">
-        <v>194</v>
+        <v>76</v>
       </c>
       <c r="S20" t="s" s="2">
         <v>76</v>
@@ -3804,11 +3790,13 @@
         <v>76</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="X20" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="X20" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="Y20" t="s" s="2">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>76</v>
@@ -3852,7 +3840,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3869,23 +3857,21 @@
         <v>76</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>200</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>76</v>
@@ -3934,7 +3920,7 @@
         <v>76</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>201</v>
+        <v>100</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>74</v>
@@ -3946,13 +3932,13 @@
         <v>76</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>76</v>
@@ -3960,18 +3946,18 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>76</v>
@@ -3983,16 +3969,16 @@
         <v>76</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>171</v>
+        <v>104</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>203</v>
+        <v>105</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>204</v>
+        <v>106</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>205</v>
+        <v>107</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -4018,49 +4004,49 @@
         <v>76</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>207</v>
+        <v>76</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>208</v>
+        <v>76</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AA22" t="s" s="2">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="AB22" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="AC22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD22" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>209</v>
+        <v>111</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>76</v>
@@ -4068,11 +4054,11 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>210</v>
+        <v>157</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>211</v>
+        <v>76</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -4088,21 +4074,23 @@
         <v>76</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>212</v>
+        <v>126</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>214</v>
+        <v>159</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="N23" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>161</v>
+      </c>
       <c r="O23" t="s" s="2">
         <v>76</v>
       </c>
@@ -4150,7 +4138,7 @@
         <v>76</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>216</v>
+        <v>162</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>74</v>
@@ -4168,7 +4156,7 @@
         <v>76</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>217</v>
+        <v>163</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>76</v>
@@ -4176,18 +4164,18 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>218</v>
+        <v>164</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>219</v>
+        <v>76</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>76</v>
@@ -4196,19 +4184,19 @@
         <v>76</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>220</v>
+        <v>86</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>223</v>
+        <v>167</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -4258,25 +4246,25 @@
         <v>76</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>224</v>
+        <v>168</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>225</v>
+        <v>169</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>76</v>
@@ -4284,7 +4272,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4292,10 +4280,10 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>76</v>
@@ -4304,25 +4292,27 @@
         <v>76</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>104</v>
+        <v>171</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>227</v>
+        <v>172</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="N25" t="s" s="2">
+        <v>174</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>76</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" t="s" s="2">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="R25" t="s" s="2">
         <v>76</v>
@@ -4352,35 +4342,37 @@
         <v>76</v>
       </c>
       <c r="AA25" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="AB25" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="AB25" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="AC25" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD25" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>76</v>
@@ -4388,11 +4380,9 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="B26" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
         <v>76</v>
       </c>
@@ -4401,7 +4391,7 @@
         <v>74</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>76</v>
@@ -4410,19 +4400,21 @@
         <v>76</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>231</v>
+        <v>86</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>232</v>
+        <v>178</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>233</v>
+        <v>179</v>
       </c>
       <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="N26" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>76</v>
       </c>
@@ -4470,25 +4462,25 @@
         <v>76</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>76</v>
@@ -4496,11 +4488,9 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="B27" t="s" s="2">
-        <v>235</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
         <v>76</v>
       </c>
@@ -4518,19 +4508,23 @@
         <v>76</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>236</v>
+        <v>184</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>237</v>
+        <v>185</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+        <v>186</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>188</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>76</v>
       </c>
@@ -4578,25 +4572,25 @@
         <v>76</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>229</v>
+        <v>189</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>76</v>
+        <v>190</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>76</v>
@@ -4604,18 +4598,18 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>76</v>
@@ -4624,23 +4618,21 @@
         <v>85</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>242</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>76</v>
       </c>
@@ -4688,33 +4680,33 @@
         <v>76</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>225</v>
+        <v>76</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4728,27 +4720,27 @@
         <v>84</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>245</v>
+        <v>171</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" t="s" s="2">
-        <v>248</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>76</v>
       </c>
@@ -4772,13 +4764,13 @@
         <v>76</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>76</v>
+        <v>205</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>76</v>
@@ -4796,7 +4788,7 @@
         <v>76</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>244</v>
+        <v>206</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>74</v>
@@ -4811,29 +4803,29 @@
         <v>96</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>249</v>
+        <v>76</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>250</v>
+        <v>76</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>251</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>76</v>
@@ -4842,21 +4834,21 @@
         <v>76</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>255</v>
+        <v>210</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" t="s" s="2">
-        <v>257</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>76</v>
       </c>
@@ -4904,13 +4896,13 @@
         <v>76</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>76</v>
@@ -4919,10 +4911,10 @@
         <v>96</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>258</v>
+        <v>76</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>76</v>
@@ -4930,11 +4922,11 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>76</v>
+        <v>216</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4950,19 +4942,19 @@
         <v>76</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>262</v>
+        <v>218</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>263</v>
+        <v>219</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>264</v>
+        <v>220</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5012,7 +5004,7 @@
         <v>76</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>74</v>
@@ -5024,57 +5016,53 @@
         <v>76</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>265</v>
+        <v>76</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>266</v>
+        <v>222</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>267</v>
+        <v>223</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>268</v>
+        <v>76</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>269</v>
+        <v>104</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>270</v>
+        <v>224</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>273</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>76</v>
       </c>
@@ -5110,37 +5098,35 @@
         <v>76</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="AB32" s="2"/>
       <c r="AC32" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>267</v>
+        <v>226</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>274</v>
+        <v>76</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>275</v>
+        <v>76</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>76</v>
@@ -5148,9 +5134,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="B33" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>227</v>
+      </c>
       <c r="C33" t="s" s="2">
         <v>76</v>
       </c>
@@ -5159,7 +5147,7 @@
         <v>74</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>76</v>
@@ -5171,13 +5159,13 @@
         <v>76</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>277</v>
+        <v>229</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5228,19 +5216,19 @@
         <v>76</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>100</v>
+        <v>226</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>76</v>
@@ -5254,9 +5242,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="B34" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>232</v>
+      </c>
       <c r="C34" t="s" s="2">
         <v>76</v>
       </c>
@@ -5265,7 +5255,7 @@
         <v>74</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>76</v>
@@ -5277,13 +5267,13 @@
         <v>76</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>104</v>
+        <v>233</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5322,17 +5312,19 @@
         <v>76</v>
       </c>
       <c r="AA34" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="AB34" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="AB34" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="AC34" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD34" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>111</v>
+        <v>226</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>74</v>
@@ -5341,7 +5333,7 @@
         <v>75</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>112</v>
@@ -5356,45 +5348,45 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="B35" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G35" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H35" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="H35" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="I35" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>281</v>
+        <v>104</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>282</v>
+        <v>237</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>239</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>76</v>
       </c>
@@ -5442,7 +5434,7 @@
         <v>76</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>111</v>
+        <v>240</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>74</v>
@@ -5451,7 +5443,7 @@
         <v>75</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>112</v>
@@ -5460,7 +5452,7 @@
         <v>76</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>76</v>
+        <v>222</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>76</v>
@@ -5468,11 +5460,9 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>285</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
         <v>76</v>
       </c>
@@ -5490,19 +5480,21 @@
         <v>76</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>286</v>
+        <v>242</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>287</v>
+        <v>243</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>288</v>
+        <v>244</v>
       </c>
       <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="N36" t="s" s="2">
+        <v>245</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>76</v>
       </c>
@@ -5550,44 +5542,44 @@
         <v>76</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>111</v>
+        <v>241</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>76</v>
+        <v>246</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>76</v>
+        <v>247</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>76</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>76</v>
@@ -5596,19 +5588,21 @@
         <v>76</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>86</v>
+        <v>251</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="N37" t="s" s="2">
+        <v>254</v>
+      </c>
       <c r="O37" t="s" s="2">
         <v>76</v>
       </c>
@@ -5656,33 +5650,33 @@
         <v>76</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>291</v>
+        <v>249</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>76</v>
+        <v>255</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>76</v>
+        <v>256</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5690,35 +5684,33 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>85</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>171</v>
+        <v>258</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>293</v>
+        <v>259</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>294</v>
+        <v>260</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>296</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>76</v>
       </c>
@@ -5742,13 +5734,13 @@
         <v>76</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>195</v>
+        <v>76</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>297</v>
+        <v>76</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>298</v>
+        <v>76</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>76</v>
@@ -5766,13 +5758,13 @@
         <v>76</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>76</v>
@@ -5781,22 +5773,22 @@
         <v>96</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>299</v>
+        <v>262</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>300</v>
+        <v>263</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>301</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5815,19 +5807,19 @@
         <v>85</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>76</v>
@@ -5876,7 +5868,7 @@
         <v>76</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>74</v>
@@ -5891,18 +5883,18 @@
         <v>96</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>311</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5922,23 +5914,19 @@
         <v>76</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>313</v>
+        <v>86</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>314</v>
+        <v>274</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>317</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>76</v>
       </c>
@@ -5986,7 +5974,7 @@
         <v>76</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>312</v>
+        <v>100</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>74</v>
@@ -5998,57 +5986,53 @@
         <v>76</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>318</v>
+        <v>76</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>319</v>
+        <v>76</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>320</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>322</v>
+        <v>76</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>323</v>
+        <v>104</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>324</v>
+        <v>224</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>327</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>76</v>
       </c>
@@ -6084,49 +6068,49 @@
         <v>76</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="AB41" s="2"/>
       <c r="AC41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD41" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>321</v>
+        <v>111</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>328</v>
+        <v>76</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>329</v>
+        <v>76</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>330</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>276</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>277</v>
+      </c>
       <c r="C42" t="s" s="2">
-        <v>332</v>
+        <v>76</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6142,23 +6126,21 @@
         <v>76</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>333</v>
+        <v>278</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>334</v>
+        <v>279</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>335</v>
+        <v>280</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>337</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>76</v>
       </c>
@@ -6206,35 +6188,37 @@
         <v>76</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>331</v>
+        <v>111</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>338</v>
+        <v>76</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>339</v>
+        <v>76</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>340</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="B43" s="2"/>
+        <v>276</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>282</v>
+      </c>
       <c r="C43" t="s" s="2">
         <v>76</v>
       </c>
@@ -6246,29 +6230,25 @@
         <v>84</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>342</v>
+        <v>283</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>343</v>
+        <v>224</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>346</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>76</v>
       </c>
@@ -6316,33 +6296,33 @@
         <v>76</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>341</v>
+        <v>111</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>347</v>
+        <v>76</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>348</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>349</v>
+        <v>284</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6353,10 +6333,10 @@
         <v>74</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>76</v>
@@ -6365,17 +6345,15 @@
         <v>76</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>350</v>
+        <v>86</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>353</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>76</v>
@@ -6424,33 +6402,33 @@
         <v>76</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>349</v>
+        <v>286</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>354</v>
+        <v>76</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>355</v>
+        <v>76</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="45" hidden="true">
+    <row r="45">
       <c r="A45" t="s" s="2">
-        <v>356</v>
+        <v>287</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6458,31 +6436,35 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F45" t="s" s="2">
         <v>84</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>98</v>
+        <v>288</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>291</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>76</v>
       </c>
@@ -6506,13 +6488,13 @@
         <v>76</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>76</v>
+        <v>292</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>76</v>
+        <v>293</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>76</v>
+        <v>294</v>
       </c>
       <c r="Z45" t="s" s="2">
         <v>76</v>
@@ -6530,10 +6512,10 @@
         <v>76</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>100</v>
+        <v>287</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>84</v>
@@ -6542,53 +6524,57 @@
         <v>76</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>76</v>
+        <v>295</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>101</v>
+        <v>296</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>76</v>
+        <v>297</v>
       </c>
     </row>
-    <row r="46" hidden="true">
+    <row r="46">
       <c r="A46" t="s" s="2">
-        <v>357</v>
+        <v>298</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>76</v>
+        <v>299</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>104</v>
+        <v>300</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>227</v>
+        <v>301</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
+        <v>302</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>304</v>
+      </c>
       <c r="O46" t="s" s="2">
         <v>76</v>
       </c>
@@ -6624,47 +6610,47 @@
         <v>76</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="AB46" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="AC46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>111</v>
+        <v>298</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>76</v>
+        <v>305</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>76</v>
+        <v>306</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>76</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>358</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
         <v>76</v>
       </c>
@@ -6682,19 +6668,23 @@
         <v>76</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>359</v>
+        <v>309</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="O47" t="s" s="2">
         <v>76</v>
       </c>
@@ -6742,67 +6732,69 @@
         <v>76</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>111</v>
+        <v>308</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>76</v>
+        <v>314</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>76</v>
+        <v>315</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>76</v>
+        <v>316</v>
       </c>
     </row>
-    <row r="48" hidden="true">
+    <row r="48">
       <c r="A48" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>362</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>76</v>
+        <v>318</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>231</v>
+        <v>319</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>232</v>
+        <v>320</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>323</v>
+      </c>
       <c r="O48" t="s" s="2">
         <v>76</v>
       </c>
@@ -6850,68 +6842,68 @@
         <v>76</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>111</v>
+        <v>317</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>76</v>
+        <v>324</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>76</v>
+        <v>325</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>76</v>
+        <v>326</v>
       </c>
     </row>
-    <row r="49" hidden="true">
+    <row r="49">
       <c r="A49" t="s" s="2">
-        <v>363</v>
+        <v>327</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>364</v>
+        <v>328</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>85</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>104</v>
+        <v>329</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>365</v>
+        <v>330</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>366</v>
+        <v>331</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>107</v>
+        <v>332</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>242</v>
+        <v>333</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>76</v>
@@ -6960,33 +6952,33 @@
         <v>76</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>367</v>
+        <v>327</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>76</v>
+        <v>334</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>225</v>
+        <v>335</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>76</v>
+        <v>336</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>368</v>
+        <v>337</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6994,32 +6986,34 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>84</v>
       </c>
       <c r="G50" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I50" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="H50" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="J50" t="s" s="2">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M50" s="2"/>
+        <v>340</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>341</v>
+      </c>
       <c r="N50" t="s" s="2">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>76</v>
@@ -7068,10 +7062,10 @@
         <v>76</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>368</v>
+        <v>337</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>84</v>
@@ -7086,15 +7080,15 @@
         <v>76</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>76</v>
+        <v>344</v>
       </c>
     </row>
-    <row r="51" hidden="true">
+    <row r="51">
       <c r="A51" t="s" s="2">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7105,10 +7099,10 @@
         <v>74</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>76</v>
@@ -7117,20 +7111,18 @@
         <v>76</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>126</v>
+        <v>346</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>377</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>76</v>
       </c>
@@ -7178,33 +7170,33 @@
         <v>76</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>96</v>
+        <v>350</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>379</v>
+        <v>352</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7218,7 +7210,7 @@
         <v>84</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>76</v>
@@ -7230,15 +7222,13 @@
         <v>86</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>380</v>
+        <v>98</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>381</v>
+        <v>99</v>
       </c>
       <c r="M52" s="2"/>
-      <c r="N52" t="s" s="2">
-        <v>382</v>
-      </c>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>76</v>
       </c>
@@ -7286,7 +7276,7 @@
         <v>76</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>379</v>
+        <v>100</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>74</v>
@@ -7298,21 +7288,21 @@
         <v>76</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>383</v>
+        <v>101</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>384</v>
+        <v>353</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7326,7 +7316,7 @@
         <v>75</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>76</v>
@@ -7335,17 +7325,15 @@
         <v>76</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>350</v>
+        <v>104</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>385</v>
+        <v>224</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>387</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>76</v>
@@ -7382,19 +7370,17 @@
         <v>76</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="AB53" s="2"/>
       <c r="AC53" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD53" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>384</v>
+        <v>111</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>74</v>
@@ -7406,13 +7392,13 @@
         <v>76</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>388</v>
+        <v>76</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>76</v>
@@ -7420,9 +7406,11 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="B54" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>354</v>
+      </c>
       <c r="C54" t="s" s="2">
         <v>76</v>
       </c>
@@ -7443,13 +7431,13 @@
         <v>76</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>86</v>
+        <v>355</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>98</v>
+        <v>356</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>99</v>
+        <v>357</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7500,25 +7488,25 @@
         <v>76</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>76</v>
@@ -7526,9 +7514,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="B55" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>358</v>
+      </c>
       <c r="C55" t="s" s="2">
         <v>76</v>
       </c>
@@ -7549,13 +7539,13 @@
         <v>76</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7594,14 +7584,16 @@
         <v>76</v>
       </c>
       <c r="AA55" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="AB55" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="AC55" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD55" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AE55" t="s" s="2">
         <v>111</v>
@@ -7613,7 +7605,7 @@
         <v>75</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>76</v>
+        <v>231</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>112</v>
@@ -7630,41 +7622,43 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="B56" t="s" s="2">
-        <v>391</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>76</v>
+        <v>360</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H56" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>392</v>
+        <v>104</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>393</v>
+        <v>361</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
+        <v>362</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>239</v>
+      </c>
       <c r="O56" t="s" s="2">
         <v>76</v>
       </c>
@@ -7712,7 +7706,7 @@
         <v>76</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>111</v>
+        <v>363</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>74</v>
@@ -7721,7 +7715,7 @@
         <v>75</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI56" t="s" s="2">
         <v>112</v>
@@ -7730,31 +7724,29 @@
         <v>76</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>76</v>
+        <v>222</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="B57" t="s" s="2">
-        <v>395</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
         <v>76</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>84</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>76</v>
@@ -7763,18 +7755,18 @@
         <v>76</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>396</v>
+        <v>86</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>397</v>
+        <v>365</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="N57" s="2"/>
+        <v>366</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" t="s" s="2">
+        <v>367</v>
+      </c>
       <c r="O57" t="s" s="2">
         <v>76</v>
       </c>
@@ -7822,25 +7814,25 @@
         <v>76</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>111</v>
+        <v>364</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>234</v>
+        <v>76</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>76</v>
+        <v>368</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>76</v>
@@ -7848,42 +7840,42 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>364</v>
+        <v>76</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
         <v>74</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H58" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>107</v>
+        <v>372</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>242</v>
+        <v>373</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>76</v>
@@ -7932,25 +7924,25 @@
         <v>76</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>225</v>
+        <v>374</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>76</v>
@@ -7958,7 +7950,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7981,19 +7973,17 @@
         <v>76</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>402</v>
+        <v>86</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>403</v>
+        <v>376</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>405</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="M59" s="2"/>
       <c r="N59" t="s" s="2">
-        <v>406</v>
+        <v>378</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>76</v>
@@ -8018,13 +8008,13 @@
         <v>76</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>407</v>
+        <v>76</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>408</v>
+        <v>76</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>76</v>
@@ -8042,7 +8032,7 @@
         <v>76</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>74</v>
@@ -8060,7 +8050,7 @@
         <v>76</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>409</v>
+        <v>379</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>76</v>
@@ -8068,7 +8058,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8091,18 +8081,18 @@
         <v>76</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>76</v>
+        <v>346</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>411</v>
+        <v>381</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="M60" s="2"/>
-      <c r="N60" t="s" s="2">
-        <v>413</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>76</v>
       </c>
@@ -8150,7 +8140,7 @@
         <v>76</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>74</v>
@@ -8168,15 +8158,15 @@
         <v>76</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>414</v>
+        <v>385</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8187,10 +8177,10 @@
         <v>74</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>76</v>
@@ -8199,18 +8189,16 @@
         <v>76</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>415</v>
+        <v>98</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>416</v>
+        <v>99</v>
       </c>
       <c r="M61" s="2"/>
-      <c r="N61" t="s" s="2">
-        <v>417</v>
-      </c>
+      <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>76</v>
       </c>
@@ -8258,32 +8246,790 @@
         <v>76</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>414</v>
+        <v>100</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AG61" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F62" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="AH61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI61" t="s" s="2">
+      <c r="G62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AB62" s="2"/>
+      <c r="AC62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" hidden="true">
+      <c r="A63" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B63" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="C63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F63" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J63" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="K63" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L63" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE63" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AF63" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG63" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH63" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AI63" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="AJ63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL63" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" hidden="true">
+      <c r="A64" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B64" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="C64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F64" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J64" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="K64" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L64" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="N64" s="2"/>
+      <c r="O64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P64" s="2"/>
+      <c r="Q64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE64" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AF64" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG64" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH64" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AI64" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="AJ64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL64" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" hidden="true">
+      <c r="A65" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F65" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H65" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="I65" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="J65" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="K65" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="O65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P65" s="2"/>
+      <c r="Q65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AL65" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F66" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G66" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="K66" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="O66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P66" s="2"/>
+      <c r="Q66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI66" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="AJ61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="AL61" t="s" s="2">
+      <c r="AJ66" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="AL66" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G67" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K67" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="O67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P67" s="2"/>
+      <c r="Q67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="F68" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G68" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="K68" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="M68" s="2"/>
+      <c r="N68" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="O68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AL68" t="s" s="2">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL61">
+  <autoFilter ref="A1:AL68">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8293,7 +9039,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI60">
+  <conditionalFormatting sqref="A2:AI67">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>